<commit_message>
finalized and tested update and merge scripts
</commit_message>
<xml_diff>
--- a/excel_files/accurates_geocoded.xlsx
+++ b/excel_files/accurates_geocoded.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for-db/excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for_db/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F6F593-6090-814A-A7D9-8BE637FD5A58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E86521-4F29-9048-B30F-40D77E1A4827}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="277">
   <si>
     <t>ADDENDUM_B_WORKSITE_ATTACHED</t>
   </si>
@@ -271,9 +271,6 @@
   </si>
   <si>
     <t>H-300-20163-645163</t>
-  </si>
-  <si>
-    <t>H-300-20119-524313</t>
   </si>
   <si>
     <t>h2visas@aol.com</t>
@@ -874,9 +871,6 @@
     <t>(44.275126, -97.773745)</t>
   </si>
   <si>
-    <t>(46.585084, -67.959887)</t>
-  </si>
-  <si>
     <t>central</t>
   </si>
   <si>
@@ -907,7 +901,22 @@
     <t>(44.335346, -97.79233)</t>
   </si>
   <si>
-    <t>(46.697136, -67.971786)</t>
+    <t>coordinates</t>
+  </si>
+  <si>
+    <t>1, 1</t>
+  </si>
+  <si>
+    <t>placeeeeee</t>
+  </si>
+  <si>
+    <t>placeeee</t>
+  </si>
+  <si>
+    <t>gibberish</t>
+  </si>
+  <si>
+    <t>H-300-20161-6388923</t>
   </si>
 </sst>
 </file>
@@ -941,12 +950,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -980,13 +995,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1328,19 +1344,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
-    <col min="17" max="19" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+    <col min="17" max="17" width="17.5" customWidth="1"/>
+    <col min="18" max="18" width="19.83203125" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" customWidth="1"/>
     <col min="21" max="21" width="8.83203125" customWidth="1"/>
-    <col min="47" max="49" width="8.83203125" customWidth="1"/>
+    <col min="47" max="47" width="8.83203125" customWidth="1"/>
+    <col min="48" max="48" width="16.33203125" customWidth="1"/>
+    <col min="49" max="49" width="8.83203125" customWidth="1"/>
     <col min="52" max="52" width="7" customWidth="1"/>
-    <col min="53" max="58" width="8.83203125" customWidth="1"/>
-    <col min="63" max="63" width="8.83203125" customWidth="1"/>
+    <col min="53" max="53" width="15" customWidth="1"/>
+    <col min="54" max="54" width="17.83203125" customWidth="1"/>
+    <col min="55" max="55" width="23" customWidth="1"/>
+    <col min="56" max="56" width="27" customWidth="1"/>
+    <col min="57" max="57" width="25.83203125" customWidth="1"/>
+    <col min="58" max="58" width="28.83203125" customWidth="1"/>
+    <col min="61" max="61" width="21.33203125" customWidth="1"/>
+    <col min="62" max="62" width="18.1640625" customWidth="1"/>
+    <col min="63" max="63" width="28.6640625" customWidth="1"/>
+    <col min="64" max="64" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" x14ac:dyDescent="0.2">
@@ -1534,7 +1563,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:64" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1554,19 +1583,19 @@
         <v>43973</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J2">
         <v>12709324115</v>
       </c>
       <c r="K2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M2" s="2">
         <v>44027</v>
@@ -1578,37 +1607,37 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="R2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="T2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W2">
         <v>6</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AA2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AB2">
         <v>15</v>
@@ -1617,22 +1646,22 @@
         <v>12704054107</v>
       </c>
       <c r="AE2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AG2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AH2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AI2" s="2">
         <v>43957</v>
       </c>
       <c r="AJ2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AK2">
         <v>6</v>
@@ -1647,61 +1676,61 @@
         <v>6</v>
       </c>
       <c r="AP2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AQ2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AR2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AS2">
         <v>12.4</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AU2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AV2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AW2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AX2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AY2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AZ2">
         <v>0</v>
       </c>
       <c r="BA2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC2">
         <v>1</v>
       </c>
       <c r="BD2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BE2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="BH2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BI2">
         <v>1</v>
       </c>
       <c r="BJ2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BK2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.2">
@@ -1724,22 +1753,22 @@
         <v>43973</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J3">
         <v>17172840111</v>
       </c>
       <c r="K3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M3" s="2">
         <v>44013</v>
@@ -1751,34 +1780,34 @@
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="T3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W3">
         <v>5</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AA3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB3">
         <v>12</v>
@@ -1787,22 +1816,22 @@
         <v>12295590241</v>
       </c>
       <c r="AE3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AF3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AH3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AI3" s="2">
         <v>43958</v>
       </c>
       <c r="AJ3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AK3">
         <v>5</v>
@@ -1817,58 +1846,58 @@
         <v>5</v>
       </c>
       <c r="AP3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AQ3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AR3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AS3">
         <v>13.34</v>
       </c>
       <c r="AU3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AV3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AW3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AX3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AY3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AZ3">
         <v>0</v>
       </c>
       <c r="BA3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BC3">
         <v>1</v>
       </c>
       <c r="BD3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BE3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BH3" t="s">
+        <v>261</v>
+      </c>
+      <c r="BI3">
+        <v>1</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>251</v>
+      </c>
+      <c r="BK3" t="s">
         <v>263</v>
-      </c>
-      <c r="BI3">
-        <v>1</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>252</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.2">
@@ -1891,19 +1920,19 @@
         <v>43973</v>
       </c>
       <c r="H4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J4">
         <v>16153899842</v>
       </c>
       <c r="K4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M4" s="2">
         <v>44032</v>
@@ -1915,34 +1944,34 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="U4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="W4">
         <v>16</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AA4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AB4">
         <v>20</v>
@@ -1951,22 +1980,22 @@
         <v>16153899842</v>
       </c>
       <c r="AE4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AF4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AG4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AH4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AI4" s="2">
         <v>43959</v>
       </c>
       <c r="AJ4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AK4">
         <v>20</v>
@@ -1981,61 +2010,61 @@
         <v>8</v>
       </c>
       <c r="AP4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AQ4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AR4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AS4">
         <v>12.4</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AU4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AV4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AW4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AX4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AY4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AZ4">
         <v>3</v>
       </c>
       <c r="BA4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BC4">
         <v>1</v>
       </c>
       <c r="BD4" t="s">
+        <v>251</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>255</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>261</v>
+      </c>
+      <c r="BI4">
+        <v>1</v>
+      </c>
+      <c r="BJ4" t="s">
         <v>252</v>
       </c>
-      <c r="BE4" t="s">
-        <v>256</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>263</v>
-      </c>
-      <c r="BI4">
-        <v>1</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>253</v>
-      </c>
       <c r="BK4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.2">
@@ -2058,19 +2087,19 @@
         <v>43973</v>
       </c>
       <c r="H5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J5">
         <v>12703452026</v>
       </c>
       <c r="K5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M5" s="2">
         <v>44032</v>
@@ -2082,34 +2111,34 @@
         <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W5">
         <v>4</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AA5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AB5">
         <v>14</v>
@@ -2118,22 +2147,22 @@
         <v>12703452026</v>
       </c>
       <c r="AE5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AF5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AG5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AH5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AI5" s="2">
         <v>43964</v>
       </c>
       <c r="AJ5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AK5">
         <v>8</v>
@@ -2148,61 +2177,61 @@
         <v>4</v>
       </c>
       <c r="AP5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AQ5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AR5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AS5">
         <v>12.4</v>
       </c>
       <c r="AT5" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AU5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AV5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AW5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AX5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AY5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AZ5">
         <v>0</v>
       </c>
       <c r="BA5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC5">
         <v>0.9</v>
       </c>
       <c r="BD5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BE5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="BH5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BI5">
         <v>0.9</v>
       </c>
       <c r="BJ5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BK5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.2">
@@ -2225,19 +2254,19 @@
         <v>43973</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J6">
         <v>15206801705</v>
       </c>
       <c r="K6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M6" s="2">
         <v>44032</v>
@@ -2249,37 +2278,37 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W6">
         <v>8</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AA6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB6">
         <v>14</v>
@@ -2288,22 +2317,22 @@
         <v>15026801705</v>
       </c>
       <c r="AE6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AG6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AH6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AI6" s="2">
         <v>43964</v>
       </c>
       <c r="AJ6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AK6">
         <v>8</v>
@@ -2318,61 +2347,61 @@
         <v>8</v>
       </c>
       <c r="AP6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AQ6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AR6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AS6">
         <v>12.4</v>
       </c>
       <c r="AT6" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AU6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AV6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AW6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AX6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AY6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AZ6">
         <v>0</v>
       </c>
       <c r="BA6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC6">
         <v>1</v>
       </c>
       <c r="BD6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BE6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BH6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BI6">
         <v>1</v>
       </c>
       <c r="BJ6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BK6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.2">
@@ -2395,19 +2424,19 @@
         <v>43973</v>
       </c>
       <c r="H7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J7">
         <v>12704024069</v>
       </c>
       <c r="K7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M7" s="2">
         <v>44022</v>
@@ -2419,37 +2448,37 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W7">
         <v>4</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AA7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB7">
         <v>15</v>
@@ -2458,22 +2487,22 @@
         <v>12704024069</v>
       </c>
       <c r="AE7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AG7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AH7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AI7" s="2">
         <v>43964</v>
       </c>
       <c r="AJ7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AK7">
         <v>10</v>
@@ -2488,61 +2517,61 @@
         <v>4</v>
       </c>
       <c r="AP7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AQ7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AR7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AS7">
         <v>12.4</v>
       </c>
       <c r="AT7" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AU7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AV7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AW7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AX7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AY7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AZ7">
         <v>0</v>
       </c>
       <c r="BA7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC7">
         <v>1</v>
       </c>
       <c r="BD7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BE7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BH7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BI7">
         <v>1</v>
       </c>
       <c r="BJ7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BK7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.2">
@@ -2565,22 +2594,22 @@
         <v>43973</v>
       </c>
       <c r="G8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J8">
         <v>17325988597</v>
       </c>
       <c r="K8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M8" s="2">
         <v>44009</v>
@@ -2592,34 +2621,34 @@
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="W8">
         <v>3</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AA8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB8">
         <v>9</v>
@@ -2628,22 +2657,22 @@
         <v>17325988597</v>
       </c>
       <c r="AE8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AF8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AG8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AH8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AI8" s="2">
         <v>43964</v>
       </c>
       <c r="AJ8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AK8">
         <v>3</v>
@@ -2658,58 +2687,58 @@
         <v>3</v>
       </c>
       <c r="AP8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AQ8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AR8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AS8">
         <v>13.34</v>
       </c>
       <c r="AU8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AV8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AW8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AX8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AY8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AZ8">
         <v>1</v>
       </c>
       <c r="BA8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="BC8">
         <v>1</v>
       </c>
       <c r="BD8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BE8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BH8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BI8">
         <v>1</v>
       </c>
       <c r="BJ8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BK8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.2">
@@ -2732,19 +2761,19 @@
         <v>43973</v>
       </c>
       <c r="H9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J9">
         <v>14024236653</v>
       </c>
       <c r="K9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M9" s="2">
         <v>44033</v>
@@ -2756,19 +2785,19 @@
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="V9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AA9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AC9">
         <v>12</v>
@@ -2780,49 +2809,49 @@
         <v>43964</v>
       </c>
       <c r="AJ9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AN9">
         <v>12</v>
       </c>
       <c r="AQ9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AS9">
         <v>25.08</v>
       </c>
       <c r="AT9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AU9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AV9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AX9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AY9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AZ9">
         <v>6</v>
       </c>
       <c r="BA9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="BH9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BI9">
         <v>1</v>
       </c>
       <c r="BJ9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BK9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.2">
@@ -2845,22 +2874,22 @@
         <v>43973</v>
       </c>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J10">
         <v>12082924290</v>
       </c>
       <c r="K10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M10" s="2">
         <v>44004</v>
@@ -2872,19 +2901,19 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="V10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AA10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AC10">
         <v>190</v>
@@ -2896,46 +2925,46 @@
         <v>43969</v>
       </c>
       <c r="AJ10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AN10">
         <v>190</v>
       </c>
       <c r="AQ10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AS10">
         <v>10.95</v>
       </c>
       <c r="AU10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AV10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AX10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AY10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AZ10">
         <v>0</v>
       </c>
       <c r="BA10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BH10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BI10">
         <v>1</v>
       </c>
       <c r="BJ10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BK10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.2">
@@ -2958,22 +2987,22 @@
         <v>43973</v>
       </c>
       <c r="G11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J11">
         <v>19109975011</v>
       </c>
       <c r="K11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M11" s="2">
         <v>44030</v>
@@ -2985,16 +3014,16 @@
         <v>1</v>
       </c>
       <c r="V11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AA11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AC11">
         <v>50</v>
@@ -3006,46 +3035,46 @@
         <v>43972</v>
       </c>
       <c r="AJ11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AN11">
         <v>50</v>
       </c>
       <c r="AQ11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AS11">
         <v>11.89</v>
       </c>
       <c r="AU11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AV11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AX11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AY11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AZ11">
         <v>3</v>
       </c>
       <c r="BA11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="BH11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BI11">
         <v>1</v>
       </c>
       <c r="BJ11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BK11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.2">
@@ -3068,22 +3097,22 @@
         <v>44007.046527777777</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J12">
         <v>16055462485</v>
       </c>
       <c r="K12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M12" s="2">
         <v>44068</v>
@@ -3095,34 +3124,34 @@
         <v>1</v>
       </c>
       <c r="Q12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="T12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="V12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W12">
         <v>10</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AA12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AB12">
         <v>14</v>
@@ -3131,16 +3160,16 @@
         <v>16055462485</v>
       </c>
       <c r="AE12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AG12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AH12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AI12" s="2">
         <v>44006</v>
@@ -3158,61 +3187,61 @@
         <v>10</v>
       </c>
       <c r="AP12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AQ12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AR12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AS12">
         <v>14.99</v>
       </c>
       <c r="AU12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AV12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AW12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AX12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AY12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AZ12">
         <v>3</v>
       </c>
       <c r="BA12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BC12">
         <v>1</v>
       </c>
       <c r="BD12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BE12" t="s">
+        <v>260</v>
+      </c>
+      <c r="BH12" t="s">
         <v>261</v>
       </c>
-      <c r="BH12" t="s">
-        <v>263</v>
-      </c>
       <c r="BI12">
         <v>1</v>
       </c>
       <c r="BJ12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BK12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:64" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3225,26 +3254,26 @@
       <c r="D13">
         <v>54</v>
       </c>
-      <c r="E13" t="s">
-        <v>83</v>
+      <c r="E13" s="4" t="s">
+        <v>276</v>
       </c>
       <c r="F13" s="2">
         <v>43973</v>
       </c>
       <c r="H13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J13">
         <v>12077644540</v>
       </c>
       <c r="K13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M13" s="2">
         <v>44021</v>
@@ -3256,37 +3285,37 @@
         <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="T13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="W13">
         <v>185</v>
       </c>
       <c r="X13" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AA13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB13">
         <v>15</v>
@@ -3295,22 +3324,22 @@
         <v>12077644540</v>
       </c>
       <c r="AE13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AF13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AG13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AH13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AI13" s="2">
         <v>43955</v>
       </c>
       <c r="AJ13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AK13">
         <v>120</v>
@@ -3325,61 +3354,70 @@
         <v>100</v>
       </c>
       <c r="AP13" t="s">
+        <v>226</v>
+      </c>
+      <c r="AQ13" t="s">
         <v>227</v>
       </c>
-      <c r="AQ13" t="s">
-        <v>228</v>
-      </c>
       <c r="AR13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AS13">
         <v>14.29</v>
       </c>
       <c r="AT13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AU13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AV13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AW13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AX13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AY13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AZ13">
         <v>3</v>
       </c>
       <c r="BA13" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="BB13" t="b">
+        <v>1</v>
       </c>
       <c r="BC13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BD13" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="BE13" t="s">
-        <v>262</v>
+        <v>272</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>271</v>
       </c>
       <c r="BH13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BI13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BJ13" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="BK13" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="BL13" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed to latitude and longitude
</commit_message>
<xml_diff>
--- a/excel_files/accurates_geocoded.xlsx
+++ b/excel_files/accurates_geocoded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for_db/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E86521-4F29-9048-B30F-40D77E1A4827}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805B1743-8AE8-FA49-9A87-BCB4AD1E4969}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="274">
   <si>
     <t>ADDENDUM_B_WORKSITE_ATTACHED</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>H-300-20163-645163</t>
+  </si>
+  <si>
+    <t>H-300-20119-524313</t>
   </si>
   <si>
     <t>h2visas@aol.com</t>
@@ -871,6 +874,9 @@
     <t>(44.275126, -97.773745)</t>
   </si>
   <si>
+    <t>(46.585084, -67.959887)</t>
+  </si>
+  <si>
     <t>central</t>
   </si>
   <si>
@@ -901,22 +907,7 @@
     <t>(44.335346, -97.79233)</t>
   </si>
   <si>
-    <t>coordinates</t>
-  </si>
-  <si>
-    <t>1, 1</t>
-  </si>
-  <si>
-    <t>placeeeeee</t>
-  </si>
-  <si>
-    <t>placeeee</t>
-  </si>
-  <si>
-    <t>gibberish</t>
-  </si>
-  <si>
-    <t>H-300-20161-6388923</t>
+    <t>(46.697136, -67.971786)</t>
   </si>
 </sst>
 </file>
@@ -950,18 +941,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -995,14 +980,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1344,32 +1328,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB13" sqref="BB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="42.6640625" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-    <col min="17" max="17" width="17.5" customWidth="1"/>
-    <col min="18" max="18" width="19.83203125" customWidth="1"/>
-    <col min="19" max="19" width="19.1640625" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
+    <col min="17" max="19" width="8.83203125" customWidth="1"/>
     <col min="21" max="21" width="8.83203125" customWidth="1"/>
-    <col min="47" max="47" width="8.83203125" customWidth="1"/>
-    <col min="48" max="48" width="16.33203125" customWidth="1"/>
-    <col min="49" max="49" width="8.83203125" customWidth="1"/>
+    <col min="47" max="49" width="8.83203125" customWidth="1"/>
     <col min="52" max="52" width="7" customWidth="1"/>
-    <col min="53" max="53" width="15" customWidth="1"/>
-    <col min="54" max="54" width="17.83203125" customWidth="1"/>
-    <col min="55" max="55" width="23" customWidth="1"/>
-    <col min="56" max="56" width="27" customWidth="1"/>
-    <col min="57" max="57" width="25.83203125" customWidth="1"/>
-    <col min="58" max="58" width="28.83203125" customWidth="1"/>
-    <col min="61" max="61" width="21.33203125" customWidth="1"/>
-    <col min="62" max="62" width="18.1640625" customWidth="1"/>
-    <col min="63" max="63" width="28.6640625" customWidth="1"/>
-    <col min="64" max="64" width="16.6640625" customWidth="1"/>
+    <col min="53" max="58" width="8.83203125" customWidth="1"/>
+    <col min="61" max="64" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" x14ac:dyDescent="0.2">
@@ -1563,7 +1535,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:64" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1583,19 +1555,19 @@
         <v>43973</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J2">
         <v>12709324115</v>
       </c>
       <c r="K2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M2" s="2">
         <v>44027</v>
@@ -1607,37 +1579,37 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="T2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="U2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="V2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="W2">
         <v>6</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AA2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AB2">
         <v>15</v>
@@ -1646,22 +1618,22 @@
         <v>12704054107</v>
       </c>
       <c r="AE2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AF2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AG2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AH2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AI2" s="2">
         <v>43957</v>
       </c>
       <c r="AJ2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AK2">
         <v>6</v>
@@ -1676,61 +1648,61 @@
         <v>6</v>
       </c>
       <c r="AP2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AQ2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AR2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AS2">
         <v>12.4</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AU2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AV2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AW2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AX2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AY2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AZ2">
         <v>0</v>
       </c>
       <c r="BA2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BC2">
         <v>1</v>
       </c>
       <c r="BD2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BE2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="BH2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI2">
         <v>1</v>
       </c>
       <c r="BJ2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BK2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.2">
@@ -1753,22 +1725,22 @@
         <v>43973</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J3">
         <v>17172840111</v>
       </c>
       <c r="K3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="M3" s="2">
         <v>44013</v>
@@ -1780,34 +1752,34 @@
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="T3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="U3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="V3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="W3">
         <v>5</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AA3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AB3">
         <v>12</v>
@@ -1816,22 +1788,22 @@
         <v>12295590241</v>
       </c>
       <c r="AE3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AF3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AG3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AH3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AI3" s="2">
         <v>43958</v>
       </c>
       <c r="AJ3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AK3">
         <v>5</v>
@@ -1846,58 +1818,58 @@
         <v>5</v>
       </c>
       <c r="AP3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AQ3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AR3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AS3">
         <v>13.34</v>
       </c>
       <c r="AU3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AV3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AW3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AX3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AY3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AZ3">
         <v>0</v>
       </c>
       <c r="BA3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC3">
         <v>1</v>
       </c>
       <c r="BD3" t="s">
+        <v>253</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>255</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>263</v>
+      </c>
+      <c r="BI3">
+        <v>1</v>
+      </c>
+      <c r="BJ3" t="s">
         <v>252</v>
       </c>
-      <c r="BE3" t="s">
-        <v>254</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>261</v>
-      </c>
-      <c r="BI3">
-        <v>1</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>251</v>
-      </c>
       <c r="BK3" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.2">
@@ -1920,19 +1892,19 @@
         <v>43973</v>
       </c>
       <c r="H4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J4">
         <v>16153899842</v>
       </c>
       <c r="K4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M4" s="2">
         <v>44032</v>
@@ -1944,34 +1916,34 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="S4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="T4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="V4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="W4">
         <v>16</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AA4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AB4">
         <v>20</v>
@@ -1980,22 +1952,22 @@
         <v>16153899842</v>
       </c>
       <c r="AE4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AF4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AG4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AH4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AI4" s="2">
         <v>43959</v>
       </c>
       <c r="AJ4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AK4">
         <v>20</v>
@@ -2010,61 +1982,61 @@
         <v>8</v>
       </c>
       <c r="AP4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AQ4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AR4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AS4">
         <v>12.4</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AU4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AV4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AW4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AX4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AY4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AZ4">
         <v>3</v>
       </c>
       <c r="BA4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="BC4">
         <v>1</v>
       </c>
       <c r="BD4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BE4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="BH4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI4">
         <v>1</v>
       </c>
       <c r="BJ4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="BK4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.2">
@@ -2087,19 +2059,19 @@
         <v>43973</v>
       </c>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J5">
         <v>12703452026</v>
       </c>
       <c r="K5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M5" s="2">
         <v>44032</v>
@@ -2111,34 +2083,34 @@
         <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="R5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="S5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="T5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="V5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="W5">
         <v>4</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AA5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AB5">
         <v>14</v>
@@ -2147,22 +2119,22 @@
         <v>12703452026</v>
       </c>
       <c r="AE5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AF5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AG5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AH5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AI5" s="2">
         <v>43964</v>
       </c>
       <c r="AJ5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AK5">
         <v>8</v>
@@ -2177,61 +2149,61 @@
         <v>4</v>
       </c>
       <c r="AP5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AQ5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AR5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AS5">
         <v>12.4</v>
       </c>
       <c r="AT5" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AU5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AV5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AW5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AX5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AY5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AZ5">
         <v>0</v>
       </c>
       <c r="BA5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BC5">
         <v>0.9</v>
       </c>
       <c r="BD5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BE5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="BH5" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI5">
         <v>0.9</v>
       </c>
       <c r="BJ5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BK5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.2">
@@ -2254,19 +2226,19 @@
         <v>43973</v>
       </c>
       <c r="H6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J6">
         <v>15206801705</v>
       </c>
       <c r="K6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M6" s="2">
         <v>44032</v>
@@ -2278,37 +2250,37 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="R6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="S6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="T6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="V6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="W6">
         <v>8</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AA6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AB6">
         <v>14</v>
@@ -2317,22 +2289,22 @@
         <v>15026801705</v>
       </c>
       <c r="AE6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AF6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AG6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AH6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AI6" s="2">
         <v>43964</v>
       </c>
       <c r="AJ6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AK6">
         <v>8</v>
@@ -2347,61 +2319,61 @@
         <v>8</v>
       </c>
       <c r="AP6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AQ6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AR6" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AS6">
         <v>12.4</v>
       </c>
       <c r="AT6" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AU6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AV6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AW6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AX6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AY6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AZ6">
         <v>0</v>
       </c>
       <c r="BA6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BC6">
         <v>1</v>
       </c>
       <c r="BD6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BE6" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="BH6" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI6">
         <v>1</v>
       </c>
       <c r="BJ6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BK6" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.2">
@@ -2424,19 +2396,19 @@
         <v>43973</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J7">
         <v>12704024069</v>
       </c>
       <c r="K7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M7" s="2">
         <v>44022</v>
@@ -2448,37 +2420,37 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="R7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="S7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="T7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="V7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="W7">
         <v>4</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AA7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AB7">
         <v>15</v>
@@ -2487,22 +2459,22 @@
         <v>12704024069</v>
       </c>
       <c r="AE7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AF7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AG7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AH7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AI7" s="2">
         <v>43964</v>
       </c>
       <c r="AJ7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AK7">
         <v>10</v>
@@ -2517,61 +2489,61 @@
         <v>4</v>
       </c>
       <c r="AP7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AQ7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AR7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AS7">
         <v>12.4</v>
       </c>
       <c r="AT7" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AU7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AV7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AW7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AX7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AY7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AZ7">
         <v>0</v>
       </c>
       <c r="BA7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BC7">
         <v>1</v>
       </c>
       <c r="BD7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BE7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="BH7" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI7">
         <v>1</v>
       </c>
       <c r="BJ7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BK7" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.2">
@@ -2594,22 +2566,22 @@
         <v>43973</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J8">
         <v>17325988597</v>
       </c>
       <c r="K8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M8" s="2">
         <v>44009</v>
@@ -2621,34 +2593,34 @@
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="R8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="S8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="T8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="U8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="V8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="W8">
         <v>3</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AA8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AB8">
         <v>9</v>
@@ -2657,22 +2629,22 @@
         <v>17325988597</v>
       </c>
       <c r="AE8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AF8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AG8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AH8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AI8" s="2">
         <v>43964</v>
       </c>
       <c r="AJ8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AK8">
         <v>3</v>
@@ -2687,58 +2659,58 @@
         <v>3</v>
       </c>
       <c r="AP8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AQ8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AR8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AS8">
         <v>13.34</v>
       </c>
       <c r="AU8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AV8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AW8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AX8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AY8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AZ8">
         <v>1</v>
       </c>
       <c r="BA8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="BC8">
         <v>1</v>
       </c>
       <c r="BD8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="BE8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="BH8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI8">
         <v>1</v>
       </c>
       <c r="BJ8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="BK8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.2">
@@ -2761,19 +2733,19 @@
         <v>43973</v>
       </c>
       <c r="H9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J9">
         <v>14024236653</v>
       </c>
       <c r="K9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M9" s="2">
         <v>44033</v>
@@ -2785,19 +2757,19 @@
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="V9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AA9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AC9">
         <v>12</v>
@@ -2809,49 +2781,49 @@
         <v>43964</v>
       </c>
       <c r="AJ9" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AN9">
         <v>12</v>
       </c>
       <c r="AQ9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AS9">
         <v>25.08</v>
       </c>
       <c r="AT9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AU9" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AV9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AX9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AY9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AZ9">
         <v>6</v>
       </c>
       <c r="BA9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="BH9" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI9">
         <v>1</v>
       </c>
       <c r="BJ9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="BK9" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.2">
@@ -2874,22 +2846,22 @@
         <v>43973</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J10">
         <v>12082924290</v>
       </c>
       <c r="K10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="M10" s="2">
         <v>44004</v>
@@ -2901,19 +2873,19 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="V10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AA10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AC10">
         <v>190</v>
@@ -2925,46 +2897,46 @@
         <v>43969</v>
       </c>
       <c r="AJ10" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AN10">
         <v>190</v>
       </c>
       <c r="AQ10" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AS10">
         <v>10.95</v>
       </c>
       <c r="AU10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AV10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AX10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AY10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AZ10">
         <v>0</v>
       </c>
       <c r="BA10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="BH10" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI10">
         <v>1</v>
       </c>
       <c r="BJ10" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="BK10" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.2">
@@ -2987,22 +2959,22 @@
         <v>43973</v>
       </c>
       <c r="G11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J11">
         <v>19109975011</v>
       </c>
       <c r="K11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M11" s="2">
         <v>44030</v>
@@ -3014,16 +2986,16 @@
         <v>1</v>
       </c>
       <c r="V11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AA11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AC11">
         <v>50</v>
@@ -3035,46 +3007,46 @@
         <v>43972</v>
       </c>
       <c r="AJ11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AN11">
         <v>50</v>
       </c>
       <c r="AQ11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AS11">
         <v>11.89</v>
       </c>
       <c r="AU11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AV11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AX11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AY11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AZ11">
         <v>3</v>
       </c>
       <c r="BA11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BH11" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI11">
         <v>1</v>
       </c>
       <c r="BJ11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="BK11" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.2">
@@ -3097,22 +3069,22 @@
         <v>44007.046527777777</v>
       </c>
       <c r="G12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J12">
         <v>16055462485</v>
       </c>
       <c r="K12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M12" s="2">
         <v>44068</v>
@@ -3124,34 +3096,34 @@
         <v>1</v>
       </c>
       <c r="Q12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="R12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="T12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="U12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="V12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="W12">
         <v>10</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AA12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AB12">
         <v>14</v>
@@ -3160,16 +3132,16 @@
         <v>16055462485</v>
       </c>
       <c r="AE12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AF12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AG12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AH12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AI12" s="2">
         <v>44006</v>
@@ -3187,61 +3159,61 @@
         <v>10</v>
       </c>
       <c r="AP12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AQ12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AR12" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AS12">
         <v>14.99</v>
       </c>
       <c r="AU12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AV12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AW12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AX12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AY12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AZ12">
         <v>3</v>
       </c>
       <c r="BA12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC12">
         <v>1</v>
       </c>
       <c r="BD12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="BE12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="BH12" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BI12">
         <v>1</v>
       </c>
       <c r="BJ12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="BK12" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:64" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3254,26 +3226,26 @@
       <c r="D13">
         <v>54</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>276</v>
+      <c r="E13" t="s">
+        <v>83</v>
       </c>
       <c r="F13" s="2">
         <v>43973</v>
       </c>
       <c r="H13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J13">
         <v>12077644540</v>
       </c>
       <c r="K13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M13" s="2">
         <v>44021</v>
@@ -3285,37 +3257,37 @@
         <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="S13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="T13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="U13" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="W13">
         <v>185</v>
       </c>
       <c r="X13" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AA13" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AB13">
         <v>15</v>
@@ -3324,22 +3296,22 @@
         <v>12077644540</v>
       </c>
       <c r="AE13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AF13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AG13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AH13" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AI13" s="2">
         <v>43955</v>
       </c>
       <c r="AJ13" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AK13">
         <v>120</v>
@@ -3354,70 +3326,64 @@
         <v>100</v>
       </c>
       <c r="AP13" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AQ13" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AR13" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AS13">
         <v>14.29</v>
       </c>
       <c r="AT13" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AU13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AV13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AW13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AX13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AY13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AZ13">
         <v>3</v>
       </c>
       <c r="BA13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BB13" t="b">
         <v>1</v>
       </c>
       <c r="BC13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BD13" t="s">
+        <v>253</v>
+      </c>
+      <c r="BE13" t="s">
+        <v>262</v>
+      </c>
+      <c r="BH13" t="s">
+        <v>263</v>
+      </c>
+      <c r="BI13">
+        <v>1</v>
+      </c>
+      <c r="BJ13" t="s">
+        <v>252</v>
+      </c>
+      <c r="BK13" t="s">
         <v>273</v>
-      </c>
-      <c r="BE13" t="s">
-        <v>272</v>
-      </c>
-      <c r="BF13" t="s">
-        <v>271</v>
-      </c>
-      <c r="BH13" t="s">
-        <v>261</v>
-      </c>
-      <c r="BI13">
-        <v>2</v>
-      </c>
-      <c r="BJ13" t="s">
-        <v>274</v>
-      </c>
-      <c r="BK13" t="s">
-        <v>272</v>
-      </c>
-      <c r="BL13" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>